<commit_message>
Genomic context from shared and top30 AMPs added
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E50781-E844-6446-B406-712EF1AE23DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D07B4-598D-E64C-AEE0-1DDB4D7CB876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5240" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4412" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4454" uniqueCount="1325">
   <si>
     <t>Seq ID</t>
   </si>
@@ -4008,6 +4008,15 @@
   </si>
   <si>
     <t>megan.blastn</t>
+  </si>
+  <si>
+    <t>genomic.context</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -4068,7 +4077,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4099,6 +4108,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4112,7 +4127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4125,6 +4140,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -52009,7 +52025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB916D6-2511-874D-B076-27DA60C31731}">
   <dimension ref="A1:E390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -65261,14 +65277,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7192636B-1268-864E-BFD4-8694A9B5E7B9}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A2:A21"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -67247,165 +67264,291 @@
       <c r="B46" s="4" t="s">
         <v>1321</v>
       </c>
+      <c r="C46" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="12" t="s">
         <v>1320</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="12" t="s">
         <v>1259</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="12" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>1000</v>
       </c>
       <c r="B50" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>1139</v>
       </c>
       <c r="B51" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>815</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="12" t="s">
         <v>1264</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>959</v>
       </c>
       <c r="B53" t="s">
         <v>1273</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>984</v>
       </c>
       <c r="B54" t="s">
         <v>1279</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>1166</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="12" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="12" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>1158</v>
       </c>
       <c r="B56" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>1002</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="12" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="12" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>1170</v>
       </c>
       <c r="B58" t="s">
         <v>1279</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="12" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>1070</v>
       </c>
       <c r="B60" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>1164</v>
       </c>
       <c r="B61" t="s">
         <v>1269</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>980</v>
       </c>
       <c r="B62" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>986</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="12" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="12" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>751</v>
       </c>
       <c r="B64" t="s">
         <v>1320</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>1057</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="12" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>936</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="12" t="s">
         <v>1317</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -67418,8 +67561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4111CD-3CDF-CF4B-987C-2E286C9BEC80}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67427,6 +67570,7 @@
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to AMPs tables
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42B4B7-D719-5542-A7A4-E463C47B16CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC832F57-3522-0D48-8632-3A8AF2E06B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="6" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3593" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="882">
   <si>
     <t>Seq ID</t>
   </si>
@@ -2682,6 +2682,12 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>AMP_134571_c44_g1_i3.p7</t>
+  </si>
+  <si>
+    <t>AMP_144878_c1_g1_i1.p9</t>
   </si>
 </sst>
 </file>
@@ -3276,7 +3282,7 @@
         <v>478</v>
       </c>
       <c r="P2">
-        <f>AVERAGE(J2:O2)</f>
+        <f t="shared" ref="P2:P33" si="0">AVERAGE(J2:O2)</f>
         <v>842.5</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -3381,7 +3387,7 @@
         <v>27</v>
       </c>
       <c r="P3">
-        <f>AVERAGE(J3:O3)</f>
+        <f t="shared" si="0"/>
         <v>782.66666666666663</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -3412,27 +3418,27 @@
         <v>361</v>
       </c>
       <c r="AB3" s="6">
-        <f t="shared" ref="AB3:AB41" si="0">VLOOKUP($AA3,$I$1:$O$194,2,FALSE)</f>
+        <f t="shared" ref="AB3:AB41" si="1">VLOOKUP($AA3,$I$1:$O$194,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="AC3" s="6">
-        <f t="shared" ref="AC3:AC41" si="1">VLOOKUP($AA3,$I$1:$O$194,3,FALSE)</f>
+        <f t="shared" ref="AC3:AC41" si="2">VLOOKUP($AA3,$I$1:$O$194,3,FALSE)</f>
         <v>29</v>
       </c>
       <c r="AD3" s="6">
-        <f t="shared" ref="AD3:AD41" si="2">VLOOKUP($AA3,$I$1:$O$194,4,FALSE)</f>
+        <f t="shared" ref="AD3:AD41" si="3">VLOOKUP($AA3,$I$1:$O$194,4,FALSE)</f>
         <v>1</v>
       </c>
       <c r="AE3" s="6">
-        <f t="shared" ref="AE3:AE41" si="3">VLOOKUP($AA3,$I$1:$O$194,5,FALSE)</f>
+        <f t="shared" ref="AE3:AE41" si="4">VLOOKUP($AA3,$I$1:$O$194,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="AF3" s="6">
-        <f t="shared" ref="AF3:AF41" si="4">VLOOKUP($AA3,$I$1:$O$194,6,FALSE)</f>
+        <f t="shared" ref="AF3:AF41" si="5">VLOOKUP($AA3,$I$1:$O$194,6,FALSE)</f>
         <v>1</v>
       </c>
       <c r="AG3" s="6">
-        <f t="shared" ref="AG3:AG41" si="5">VLOOKUP($AA3,$I$1:$O$194,7,FALSE)</f>
+        <f t="shared" ref="AG3:AG41" si="6">VLOOKUP($AA3,$I$1:$O$194,7,FALSE)</f>
         <v>2</v>
       </c>
     </row>
@@ -3486,7 +3492,7 @@
         <v>25</v>
       </c>
       <c r="P4">
-        <f>AVERAGE(J4:O4)</f>
+        <f t="shared" si="0"/>
         <v>593.5</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -3517,27 +3523,27 @@
         <v>544</v>
       </c>
       <c r="AB4" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="AC4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AD4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="AE4" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF4" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG4" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3591,7 +3597,7 @@
         <v>10</v>
       </c>
       <c r="P5">
-        <f>AVERAGE(J5:O5)</f>
+        <f t="shared" si="0"/>
         <v>323.83333333333331</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -3622,27 +3628,27 @@
         <v>498</v>
       </c>
       <c r="AB5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="AC5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="AE5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG5" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -3696,7 +3702,7 @@
         <v>748</v>
       </c>
       <c r="P6">
-        <f>AVERAGE(J6:O6)</f>
+        <f t="shared" si="0"/>
         <v>317.83333333333331</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -3727,27 +3733,27 @@
         <v>424</v>
       </c>
       <c r="AB6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="AC6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="AD6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE6" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AF6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG6" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -3801,7 +3807,7 @@
         <v>3</v>
       </c>
       <c r="P7">
-        <f>AVERAGE(J7:O7)</f>
+        <f t="shared" si="0"/>
         <v>289.5</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -3832,27 +3838,27 @@
         <v>627</v>
       </c>
       <c r="AB7" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="AC7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG7" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -3906,7 +3912,7 @@
         <v>61</v>
       </c>
       <c r="P8">
-        <f>AVERAGE(J8:O8)</f>
+        <f t="shared" si="0"/>
         <v>233.16666666666666</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -3937,27 +3943,27 @@
         <v>409</v>
       </c>
       <c r="AB8" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AF8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG8" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
@@ -4011,7 +4017,7 @@
         <v>23</v>
       </c>
       <c r="P9">
-        <f>AVERAGE(J9:O9)</f>
+        <f t="shared" si="0"/>
         <v>182.33333333333334</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -4042,27 +4048,27 @@
         <v>546</v>
       </c>
       <c r="AB9" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="AF9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG9" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
     </row>
@@ -4116,7 +4122,7 @@
         <v>419</v>
       </c>
       <c r="P10">
-        <f>AVERAGE(J10:O10)</f>
+        <f t="shared" si="0"/>
         <v>152.66666666666666</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -4147,27 +4153,27 @@
         <v>762</v>
       </c>
       <c r="AB10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="AG10" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -4221,7 +4227,7 @@
         <v>307</v>
       </c>
       <c r="P11">
-        <f>AVERAGE(J11:O11)</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -4252,27 +4258,27 @@
         <v>527</v>
       </c>
       <c r="AB11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="AF11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG11" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
     </row>
@@ -4326,7 +4332,7 @@
         <v>95</v>
       </c>
       <c r="P12">
-        <f>AVERAGE(J12:O12)</f>
+        <f t="shared" si="0"/>
         <v>122.33333333333333</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -4357,27 +4363,27 @@
         <v>395</v>
       </c>
       <c r="AB12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="AF12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
     </row>
@@ -4431,7 +4437,7 @@
         <v>106</v>
       </c>
       <c r="P13">
-        <f>AVERAGE(J13:O13)</f>
+        <f t="shared" si="0"/>
         <v>106.16666666666667</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -4462,27 +4468,27 @@
         <v>435</v>
       </c>
       <c r="AB13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="AC13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="AF13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG13" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -4536,7 +4542,7 @@
         <v>12</v>
       </c>
       <c r="P14">
-        <f>AVERAGE(J14:O14)</f>
+        <f t="shared" si="0"/>
         <v>105.83333333333333</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -4567,27 +4573,27 @@
         <v>513</v>
       </c>
       <c r="AB14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC14" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="AF14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG14" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -4641,7 +4647,7 @@
         <v>6</v>
       </c>
       <c r="P15">
-        <f>AVERAGE(J15:O15)</f>
+        <f t="shared" si="0"/>
         <v>105.5</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -4672,27 +4678,27 @@
         <v>607</v>
       </c>
       <c r="AB15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AC15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="AG15" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4746,7 +4752,7 @@
         <v>155</v>
       </c>
       <c r="P16">
-        <f>AVERAGE(J16:O16)</f>
+        <f t="shared" si="0"/>
         <v>100.66666666666667</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -4777,27 +4783,27 @@
         <v>562</v>
       </c>
       <c r="AB16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AC16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="AE16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="AF16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
     </row>
@@ -4851,7 +4857,7 @@
         <v>7</v>
       </c>
       <c r="P17">
-        <f>AVERAGE(J17:O17)</f>
+        <f t="shared" si="0"/>
         <v>100.33333333333333</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -4882,27 +4888,27 @@
         <v>668</v>
       </c>
       <c r="AB17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="AG17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
     </row>
@@ -4956,7 +4962,7 @@
         <v>32</v>
       </c>
       <c r="P18">
-        <f>AVERAGE(J18:O18)</f>
+        <f t="shared" si="0"/>
         <v>97.666666666666671</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -4987,27 +4993,27 @@
         <v>638</v>
       </c>
       <c r="AB18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="AC18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="AE18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>408</v>
       </c>
       <c r="AF18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="AG18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>307</v>
       </c>
     </row>
@@ -5061,7 +5067,7 @@
         <v>3</v>
       </c>
       <c r="P19">
-        <f>AVERAGE(J19:O19)</f>
+        <f t="shared" si="0"/>
         <v>78.166666666666671</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -5092,27 +5098,27 @@
         <v>352</v>
       </c>
       <c r="AB19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AC19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="AE19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF19" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="AG19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
@@ -5166,7 +5172,7 @@
         <v>5</v>
       </c>
       <c r="P20">
-        <f>AVERAGE(J20:O20)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -5197,27 +5203,27 @@
         <v>341</v>
       </c>
       <c r="AB20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="AC20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF20" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="AG20" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -5271,7 +5277,7 @@
         <v>179</v>
       </c>
       <c r="P21">
-        <f>AVERAGE(J21:O21)</f>
+        <f t="shared" si="0"/>
         <v>71.833333333333329</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -5302,27 +5308,27 @@
         <v>346</v>
       </c>
       <c r="AB21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AC21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AD21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="AE21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>420</v>
       </c>
       <c r="AF21" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG21" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>155</v>
       </c>
     </row>
@@ -5376,7 +5382,7 @@
         <v>32</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(J22:O22)</f>
+        <f t="shared" si="0"/>
         <v>61.666666666666664</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -5407,27 +5413,27 @@
         <v>584</v>
       </c>
       <c r="AB22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF22" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="AG22" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -5481,7 +5487,7 @@
         <v>39</v>
       </c>
       <c r="P23">
-        <f>AVERAGE(J23:O23)</f>
+        <f t="shared" si="0"/>
         <v>57.833333333333336</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -5512,27 +5518,27 @@
         <v>655</v>
       </c>
       <c r="AB23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="AF23" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="AG23" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
@@ -5586,7 +5592,7 @@
         <v>15</v>
       </c>
       <c r="P24">
-        <f>AVERAGE(J24:O24)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -5617,27 +5623,27 @@
         <v>534</v>
       </c>
       <c r="AB24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
       <c r="AF24" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG24" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
     </row>
@@ -5691,7 +5697,7 @@
         <v>3</v>
       </c>
       <c r="P25">
-        <f>AVERAGE(J25:O25)</f>
+        <f t="shared" si="0"/>
         <v>50.333333333333336</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -5722,27 +5728,27 @@
         <v>370</v>
       </c>
       <c r="AB25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="AC25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AE25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>514</v>
       </c>
       <c r="AF25" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG25" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
     </row>
@@ -5796,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="P26">
-        <f>AVERAGE(J26:O26)</f>
+        <f t="shared" si="0"/>
         <v>47.166666666666664</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -5827,27 +5833,27 @@
         <v>413</v>
       </c>
       <c r="AB26" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="AC26" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AD26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="AE26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4480</v>
       </c>
       <c r="AF26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG26" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>478</v>
       </c>
     </row>
@@ -5901,7 +5907,7 @@
         <v>19</v>
       </c>
       <c r="P27">
-        <f>AVERAGE(J27:O27)</f>
+        <f t="shared" si="0"/>
         <v>44.333333333333336</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -5932,27 +5938,27 @@
         <v>515</v>
       </c>
       <c r="AB27" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="AC27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="AD27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="AE27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="AF27" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AG27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
     </row>
@@ -6006,7 +6012,7 @@
         <v>64</v>
       </c>
       <c r="P28">
-        <f>AVERAGE(J28:O28)</f>
+        <f t="shared" si="0"/>
         <v>41.5</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -6037,27 +6043,27 @@
         <v>616</v>
       </c>
       <c r="AB28" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>213</v>
       </c>
       <c r="AC28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="AD28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="AE28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>742</v>
       </c>
       <c r="AF28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="AG28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>748</v>
       </c>
     </row>
@@ -6111,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <f>AVERAGE(J29:O29)</f>
+        <f t="shared" si="0"/>
         <v>38.833333333333336</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -6142,27 +6148,27 @@
         <v>515</v>
       </c>
       <c r="AB29" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="AC29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="AD29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="AE29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="AF29" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AG29" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
     </row>
@@ -6216,7 +6222,7 @@
         <v>3</v>
       </c>
       <c r="P30">
-        <f>AVERAGE(J30:O30)</f>
+        <f t="shared" si="0"/>
         <v>38.333333333333336</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -6247,27 +6253,27 @@
         <v>616</v>
       </c>
       <c r="AB30" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>213</v>
       </c>
       <c r="AC30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="AD30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="AE30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>742</v>
       </c>
       <c r="AF30" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="AG30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>748</v>
       </c>
     </row>
@@ -6321,7 +6327,7 @@
         <v>11</v>
       </c>
       <c r="P31">
-        <f>AVERAGE(J31:O31)</f>
+        <f t="shared" si="0"/>
         <v>35.166666666666664</v>
       </c>
       <c r="R31" s="3" t="s">
@@ -6352,27 +6358,27 @@
         <v>511</v>
       </c>
       <c r="AB31" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="AC31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="AE31" s="6">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AF31" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
+      <c r="AF31" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="AG31" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -6426,7 +6432,7 @@
         <v>183</v>
       </c>
       <c r="P32">
-        <f>AVERAGE(J32:O32)</f>
+        <f t="shared" si="0"/>
         <v>35.166666666666664</v>
       </c>
       <c r="R32" s="3" t="s">
@@ -6457,27 +6463,27 @@
         <v>687</v>
       </c>
       <c r="AB32" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="AC32" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="AF32" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AG32" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
@@ -6531,7 +6537,7 @@
         <v>51</v>
       </c>
       <c r="P33">
-        <f>AVERAGE(J33:O33)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="R33" s="3" t="s">
@@ -6562,27 +6568,27 @@
         <v>413</v>
       </c>
       <c r="AB33" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="AC33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AD33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="AE33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4480</v>
       </c>
       <c r="AF33" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG33" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>478</v>
       </c>
     </row>
@@ -6636,7 +6642,7 @@
         <v>1</v>
       </c>
       <c r="P34">
-        <f>AVERAGE(J34:O34)</f>
+        <f t="shared" ref="P34:P65" si="7">AVERAGE(J34:O34)</f>
         <v>31.5</v>
       </c>
       <c r="R34" s="3" t="s">
@@ -6667,27 +6673,27 @@
         <v>604</v>
       </c>
       <c r="AB34" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
       <c r="AC34" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="AD34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE34" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF34" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="AG34" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -6741,7 +6747,7 @@
         <v>39</v>
       </c>
       <c r="P35">
-        <f>AVERAGE(J35:O35)</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="R35" s="3" t="s">
@@ -6772,27 +6778,27 @@
         <v>375</v>
       </c>
       <c r="AB35" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="AC35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="AD35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="AG35" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -6846,7 +6852,7 @@
         <v>14</v>
       </c>
       <c r="P36">
-        <f>AVERAGE(J36:O36)</f>
+        <f t="shared" si="7"/>
         <v>28.666666666666668</v>
       </c>
       <c r="R36" s="3" t="s">
@@ -6877,27 +6883,27 @@
         <v>638</v>
       </c>
       <c r="AB36" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="AC36" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="AE36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>408</v>
       </c>
       <c r="AF36" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="AG36" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>307</v>
       </c>
     </row>
@@ -6951,7 +6957,7 @@
         <v>25</v>
       </c>
       <c r="P37">
-        <f>AVERAGE(J37:O37)</f>
+        <f t="shared" si="7"/>
         <v>28.166666666666668</v>
       </c>
       <c r="R37" s="3" t="s">
@@ -6982,27 +6988,27 @@
         <v>461</v>
       </c>
       <c r="AB37" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AC37" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AD37" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="AD37" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="AE37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="AF37" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG37" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -7056,7 +7062,7 @@
         <v>14</v>
       </c>
       <c r="P38">
-        <f>AVERAGE(J38:O38)</f>
+        <f t="shared" si="7"/>
         <v>27.666666666666668</v>
       </c>
       <c r="R38" s="3" t="s">
@@ -7087,27 +7093,27 @@
         <v>346</v>
       </c>
       <c r="AB38" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AC38" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AD38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="AE38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>420</v>
       </c>
       <c r="AF38" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG38" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>155</v>
       </c>
     </row>
@@ -7161,7 +7167,7 @@
         <v>131</v>
       </c>
       <c r="P39">
-        <f>AVERAGE(J39:O39)</f>
+        <f t="shared" si="7"/>
         <v>26.833333333333332</v>
       </c>
       <c r="R39" s="3" t="s">
@@ -7192,27 +7198,27 @@
         <v>538</v>
       </c>
       <c r="AB39" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="AC39" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="AD39" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="AE39" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="AF39" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
@@ -7266,7 +7272,7 @@
         <v>11</v>
       </c>
       <c r="P40">
-        <f>AVERAGE(J40:O40)</f>
+        <f t="shared" si="7"/>
         <v>25.666666666666668</v>
       </c>
       <c r="R40" s="3" t="s">
@@ -7297,27 +7303,27 @@
         <v>463</v>
       </c>
       <c r="AB40" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="AC40" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD40" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AE40" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="AF40" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AG40" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
     </row>
@@ -7371,7 +7377,7 @@
         <v>46</v>
       </c>
       <c r="P41">
-        <f>AVERAGE(J41:O41)</f>
+        <f t="shared" si="7"/>
         <v>25.166666666666668</v>
       </c>
       <c r="R41" s="3" t="s">
@@ -7402,27 +7408,27 @@
         <v>412</v>
       </c>
       <c r="AB41" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="AC41" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD41" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="AE41" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="AF41" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="AG41" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -7476,7 +7482,7 @@
         <v>1</v>
       </c>
       <c r="P42">
-        <f>AVERAGE(J42:O42)</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="R42" s="3" t="s">
@@ -7554,7 +7560,7 @@
         <v>5</v>
       </c>
       <c r="P43">
-        <f>AVERAGE(J43:O43)</f>
+        <f t="shared" si="7"/>
         <v>24.833333333333332</v>
       </c>
       <c r="R43" s="3" t="s">
@@ -7632,7 +7638,7 @@
         <v>9</v>
       </c>
       <c r="P44">
-        <f>AVERAGE(J44:O44)</f>
+        <f t="shared" si="7"/>
         <v>24.666666666666668</v>
       </c>
       <c r="R44" s="3" t="s">
@@ -7710,7 +7716,7 @@
         <v>12</v>
       </c>
       <c r="P45">
-        <f>AVERAGE(J45:O45)</f>
+        <f t="shared" si="7"/>
         <v>23.166666666666668</v>
       </c>
       <c r="R45" s="3" t="s">
@@ -7788,7 +7794,7 @@
         <v>15</v>
       </c>
       <c r="P46">
-        <f>AVERAGE(J46:O46)</f>
+        <f t="shared" si="7"/>
         <v>22.833333333333332</v>
       </c>
       <c r="R46" s="3" t="s">
@@ -7866,7 +7872,7 @@
         <v>9</v>
       </c>
       <c r="P47">
-        <f>AVERAGE(J47:O47)</f>
+        <f t="shared" si="7"/>
         <v>20.666666666666668</v>
       </c>
       <c r="R47" s="3" t="s">
@@ -7944,7 +7950,7 @@
         <v>18</v>
       </c>
       <c r="P48">
-        <f>AVERAGE(J48:O48)</f>
+        <f t="shared" si="7"/>
         <v>20.666666666666668</v>
       </c>
       <c r="R48" s="3" t="s">
@@ -8022,7 +8028,7 @@
         <v>1</v>
       </c>
       <c r="P49">
-        <f>AVERAGE(J49:O49)</f>
+        <f t="shared" si="7"/>
         <v>20.166666666666668</v>
       </c>
       <c r="R49" s="3" t="s">
@@ -8100,7 +8106,7 @@
         <v>14</v>
       </c>
       <c r="P50">
-        <f>AVERAGE(J50:O50)</f>
+        <f t="shared" si="7"/>
         <v>19.833333333333332</v>
       </c>
       <c r="R50" s="3" t="s">
@@ -8178,7 +8184,7 @@
         <v>50</v>
       </c>
       <c r="P51">
-        <f>AVERAGE(J51:O51)</f>
+        <f t="shared" si="7"/>
         <v>19.5</v>
       </c>
       <c r="R51" s="3" t="s">
@@ -8256,7 +8262,7 @@
         <v>4</v>
       </c>
       <c r="P52">
-        <f>AVERAGE(J52:O52)</f>
+        <f t="shared" si="7"/>
         <v>17.5</v>
       </c>
       <c r="R52" s="3" t="s">
@@ -8334,7 +8340,7 @@
         <v>74</v>
       </c>
       <c r="P53">
-        <f>AVERAGE(J53:O53)</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="R53" s="3" t="s">
@@ -8412,7 +8418,7 @@
         <v>41</v>
       </c>
       <c r="P54">
-        <f>AVERAGE(J54:O54)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="R54" s="3" t="s">
@@ -8490,7 +8496,7 @@
         <v>45</v>
       </c>
       <c r="P55">
-        <f>AVERAGE(J55:O55)</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="R55" s="3" t="s">
@@ -8568,7 +8574,7 @@
         <v>9</v>
       </c>
       <c r="P56">
-        <f>AVERAGE(J56:O56)</f>
+        <f t="shared" si="7"/>
         <v>14.833333333333334</v>
       </c>
       <c r="R56" s="3" t="s">
@@ -8646,7 +8652,7 @@
         <v>21</v>
       </c>
       <c r="P57">
-        <f>AVERAGE(J57:O57)</f>
+        <f t="shared" si="7"/>
         <v>14.666666666666666</v>
       </c>
       <c r="R57" s="3" t="s">
@@ -8724,7 +8730,7 @@
         <v>28</v>
       </c>
       <c r="P58">
-        <f>AVERAGE(J58:O58)</f>
+        <f t="shared" si="7"/>
         <v>13.833333333333334</v>
       </c>
       <c r="R58" s="3" t="s">
@@ -8802,7 +8808,7 @@
         <v>31</v>
       </c>
       <c r="P59">
-        <f>AVERAGE(J59:O59)</f>
+        <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
       <c r="R59" s="3" t="s">
@@ -8880,7 +8886,7 @@
         <v>50</v>
       </c>
       <c r="P60">
-        <f>AVERAGE(J60:O60)</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="R60" s="3" t="s">
@@ -8958,7 +8964,7 @@
         <v>27</v>
       </c>
       <c r="P61">
-        <f>AVERAGE(J61:O61)</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="R61" s="3" t="s">
@@ -9036,7 +9042,7 @@
         <v>11</v>
       </c>
       <c r="P62">
-        <f>AVERAGE(J62:O62)</f>
+        <f t="shared" si="7"/>
         <v>11.833333333333334</v>
       </c>
       <c r="R62" s="3" t="s">
@@ -9114,7 +9120,7 @@
         <v>3</v>
       </c>
       <c r="P63">
-        <f>AVERAGE(J63:O63)</f>
+        <f t="shared" si="7"/>
         <v>11.666666666666666</v>
       </c>
       <c r="R63" s="3" t="s">
@@ -9192,7 +9198,7 @@
         <v>20</v>
       </c>
       <c r="P64">
-        <f>AVERAGE(J64:O64)</f>
+        <f t="shared" si="7"/>
         <v>11.333333333333334</v>
       </c>
       <c r="R64" s="3" t="s">
@@ -9270,7 +9276,7 @@
         <v>29</v>
       </c>
       <c r="P65">
-        <f>AVERAGE(J65:O65)</f>
+        <f t="shared" si="7"/>
         <v>10.833333333333334</v>
       </c>
       <c r="R65" s="3" t="s">
@@ -9348,7 +9354,7 @@
         <v>44</v>
       </c>
       <c r="P66">
-        <f>AVERAGE(J66:O66)</f>
+        <f t="shared" ref="P66:P97" si="8">AVERAGE(J66:O66)</f>
         <v>10.833333333333334</v>
       </c>
       <c r="R66" s="3" t="s">
@@ -9426,7 +9432,7 @@
         <v>47</v>
       </c>
       <c r="P67">
-        <f>AVERAGE(J67:O67)</f>
+        <f t="shared" si="8"/>
         <v>10.333333333333334</v>
       </c>
       <c r="R67" s="3" t="s">
@@ -9504,7 +9510,7 @@
         <v>9</v>
       </c>
       <c r="P68">
-        <f>AVERAGE(J68:O68)</f>
+        <f t="shared" si="8"/>
         <v>10.166666666666666</v>
       </c>
       <c r="R68" s="3" t="s">
@@ -9582,7 +9588,7 @@
         <v>2</v>
       </c>
       <c r="P69">
-        <f>AVERAGE(J69:O69)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="R69" s="3" t="s">
@@ -9660,7 +9666,7 @@
         <v>3</v>
       </c>
       <c r="P70">
-        <f>AVERAGE(J70:O70)</f>
+        <f t="shared" si="8"/>
         <v>9.6666666666666661</v>
       </c>
       <c r="R70" s="3" t="s">
@@ -9738,7 +9744,7 @@
         <v>5</v>
       </c>
       <c r="P71">
-        <f>AVERAGE(J71:O71)</f>
+        <f t="shared" si="8"/>
         <v>8.8333333333333339</v>
       </c>
       <c r="R71" s="3" t="s">
@@ -9816,7 +9822,7 @@
         <v>29</v>
       </c>
       <c r="P72">
-        <f>AVERAGE(J72:O72)</f>
+        <f t="shared" si="8"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="R72" s="3" t="s">
@@ -9894,7 +9900,7 @@
         <v>21</v>
       </c>
       <c r="P73">
-        <f>AVERAGE(J73:O73)</f>
+        <f t="shared" si="8"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="R73" s="3" t="s">
@@ -9972,7 +9978,7 @@
         <v>3</v>
       </c>
       <c r="P74">
-        <f>AVERAGE(J74:O74)</f>
+        <f t="shared" si="8"/>
         <v>8.1666666666666661</v>
       </c>
       <c r="R74" s="3" t="s">
@@ -10050,7 +10056,7 @@
         <v>10</v>
       </c>
       <c r="P75">
-        <f>AVERAGE(J75:O75)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="R75" s="3" t="s">
@@ -10128,7 +10134,7 @@
         <v>5</v>
       </c>
       <c r="P76">
-        <f>AVERAGE(J76:O76)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="R76" s="3" t="s">
@@ -10206,7 +10212,7 @@
         <v>1</v>
       </c>
       <c r="P77">
-        <f>AVERAGE(J77:O77)</f>
+        <f t="shared" si="8"/>
         <v>7.666666666666667</v>
       </c>
       <c r="R77" s="3" t="s">
@@ -10284,7 +10290,7 @@
         <v>5</v>
       </c>
       <c r="P78">
-        <f>AVERAGE(J78:O78)</f>
+        <f t="shared" si="8"/>
         <v>7.5</v>
       </c>
       <c r="R78" s="3" t="s">
@@ -10362,7 +10368,7 @@
         <v>2</v>
       </c>
       <c r="P79">
-        <f>AVERAGE(J79:O79)</f>
+        <f t="shared" si="8"/>
         <v>7.166666666666667</v>
       </c>
       <c r="R79" s="3" t="s">
@@ -10440,7 +10446,7 @@
         <v>3</v>
       </c>
       <c r="P80">
-        <f>AVERAGE(J80:O80)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="R80" s="3" t="s">
@@ -10518,7 +10524,7 @@
         <v>2</v>
       </c>
       <c r="P81">
-        <f>AVERAGE(J81:O81)</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="R81" s="3" t="s">
@@ -10596,7 +10602,7 @@
         <v>1</v>
       </c>
       <c r="P82">
-        <f>AVERAGE(J82:O82)</f>
+        <f t="shared" si="8"/>
         <v>6.833333333333333</v>
       </c>
       <c r="R82" s="3" t="s">
@@ -10674,7 +10680,7 @@
         <v>9</v>
       </c>
       <c r="P83">
-        <f>AVERAGE(J83:O83)</f>
+        <f t="shared" si="8"/>
         <v>6.666666666666667</v>
       </c>
       <c r="R83" s="3" t="s">
@@ -10752,7 +10758,7 @@
         <v>2</v>
       </c>
       <c r="P84">
-        <f>AVERAGE(J84:O84)</f>
+        <f t="shared" si="8"/>
         <v>6.666666666666667</v>
       </c>
       <c r="R84" s="3" t="s">
@@ -10830,7 +10836,7 @@
         <v>3</v>
       </c>
       <c r="P85">
-        <f>AVERAGE(J85:O85)</f>
+        <f t="shared" si="8"/>
         <v>6.5</v>
       </c>
       <c r="R85" s="3" t="s">
@@ -10908,7 +10914,7 @@
         <v>1</v>
       </c>
       <c r="P86">
-        <f>AVERAGE(J86:O86)</f>
+        <f t="shared" si="8"/>
         <v>6.5</v>
       </c>
       <c r="R86" s="3" t="s">
@@ -10986,7 +10992,7 @@
         <v>1</v>
       </c>
       <c r="P87">
-        <f>AVERAGE(J87:O87)</f>
+        <f t="shared" si="8"/>
         <v>6.5</v>
       </c>
       <c r="R87" s="3" t="s">
@@ -11064,7 +11070,7 @@
         <v>30</v>
       </c>
       <c r="P88">
-        <f>AVERAGE(J88:O88)</f>
+        <f t="shared" si="8"/>
         <v>6.333333333333333</v>
       </c>
       <c r="R88" s="3" t="s">
@@ -11142,7 +11148,7 @@
         <v>2</v>
       </c>
       <c r="P89">
-        <f>AVERAGE(J89:O89)</f>
+        <f t="shared" si="8"/>
         <v>6.333333333333333</v>
       </c>
       <c r="R89" s="3" t="s">
@@ -11220,7 +11226,7 @@
         <v>7</v>
       </c>
       <c r="P90">
-        <f>AVERAGE(J90:O90)</f>
+        <f t="shared" si="8"/>
         <v>6.166666666666667</v>
       </c>
       <c r="R90" s="3" t="s">
@@ -11298,7 +11304,7 @@
         <v>17</v>
       </c>
       <c r="P91">
-        <f>AVERAGE(J91:O91)</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="R91" s="3" t="s">
@@ -11376,7 +11382,7 @@
         <v>30</v>
       </c>
       <c r="P92">
-        <f>AVERAGE(J92:O92)</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="R92" s="3" t="s">
@@ -11454,7 +11460,7 @@
         <v>1</v>
       </c>
       <c r="P93">
-        <f>AVERAGE(J93:O93)</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="R93" s="3" t="s">
@@ -11532,7 +11538,7 @@
         <v>2</v>
       </c>
       <c r="P94">
-        <f>AVERAGE(J94:O94)</f>
+        <f t="shared" si="8"/>
         <v>5.833333333333333</v>
       </c>
       <c r="R94" s="3" t="s">
@@ -11610,7 +11616,7 @@
         <v>11</v>
       </c>
       <c r="P95">
-        <f>AVERAGE(J95:O95)</f>
+        <f t="shared" si="8"/>
         <v>5.833333333333333</v>
       </c>
       <c r="R95" s="3" t="s">
@@ -11688,7 +11694,7 @@
         <v>19</v>
       </c>
       <c r="P96">
-        <f>AVERAGE(J96:O96)</f>
+        <f t="shared" si="8"/>
         <v>5.666666666666667</v>
       </c>
       <c r="R96" s="3" t="s">
@@ -11766,7 +11772,7 @@
         <v>13</v>
       </c>
       <c r="P97">
-        <f>AVERAGE(J97:O97)</f>
+        <f t="shared" si="8"/>
         <v>5.666666666666667</v>
       </c>
       <c r="R97" s="3" t="s">
@@ -11844,7 +11850,7 @@
         <v>4</v>
       </c>
       <c r="P98">
-        <f>AVERAGE(J98:O98)</f>
+        <f t="shared" ref="P98:P129" si="9">AVERAGE(J98:O98)</f>
         <v>5.666666666666667</v>
       </c>
       <c r="R98" s="3" t="s">
@@ -11922,7 +11928,7 @@
         <v>23</v>
       </c>
       <c r="P99">
-        <f>AVERAGE(J99:O99)</f>
+        <f t="shared" si="9"/>
         <v>5.666666666666667</v>
       </c>
       <c r="R99" s="3" t="s">
@@ -12000,7 +12006,7 @@
         <v>15</v>
       </c>
       <c r="P100">
-        <f>AVERAGE(J100:O100)</f>
+        <f t="shared" si="9"/>
         <v>5.666666666666667</v>
       </c>
       <c r="R100" s="3" t="s">
@@ -12078,7 +12084,7 @@
         <v>25</v>
       </c>
       <c r="P101">
-        <f>AVERAGE(J101:O101)</f>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="R101" s="3" t="s">
@@ -12156,7 +12162,7 @@
         <v>18</v>
       </c>
       <c r="P102">
-        <f>AVERAGE(J102:O102)</f>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="R102" s="3" t="s">
@@ -12234,7 +12240,7 @@
         <v>5</v>
       </c>
       <c r="P103">
-        <f>AVERAGE(J103:O103)</f>
+        <f t="shared" si="9"/>
         <v>5.333333333333333</v>
       </c>
       <c r="R103" s="3" t="s">
@@ -12312,7 +12318,7 @@
         <v>5</v>
       </c>
       <c r="P104">
-        <f>AVERAGE(J104:O104)</f>
+        <f t="shared" si="9"/>
         <v>5.166666666666667</v>
       </c>
       <c r="R104" s="3" t="s">
@@ -12390,7 +12396,7 @@
         <v>5</v>
       </c>
       <c r="P105">
-        <f>AVERAGE(J105:O105)</f>
+        <f t="shared" si="9"/>
         <v>5.166666666666667</v>
       </c>
       <c r="R105" s="3" t="s">
@@ -12468,7 +12474,7 @@
         <v>25</v>
       </c>
       <c r="P106">
-        <f>AVERAGE(J106:O106)</f>
+        <f t="shared" si="9"/>
         <v>5.166666666666667</v>
       </c>
       <c r="R106" s="3" t="s">
@@ -12546,7 +12552,7 @@
         <v>14</v>
       </c>
       <c r="P107">
-        <f>AVERAGE(J107:O107)</f>
+        <f t="shared" si="9"/>
         <v>5.166666666666667</v>
       </c>
       <c r="R107" s="3" t="s">
@@ -12624,7 +12630,7 @@
         <v>2</v>
       </c>
       <c r="P108">
-        <f>AVERAGE(J108:O108)</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="R108" s="3" t="s">
@@ -12702,7 +12708,7 @@
         <v>2</v>
       </c>
       <c r="P109">
-        <f>AVERAGE(J109:O109)</f>
+        <f t="shared" si="9"/>
         <v>4.666666666666667</v>
       </c>
       <c r="R109" s="3" t="s">
@@ -12780,7 +12786,7 @@
         <v>9</v>
       </c>
       <c r="P110">
-        <f>AVERAGE(J110:O110)</f>
+        <f t="shared" si="9"/>
         <v>4.5</v>
       </c>
       <c r="R110" s="3" t="s">
@@ -12858,7 +12864,7 @@
         <v>20</v>
       </c>
       <c r="P111">
-        <f>AVERAGE(J111:O111)</f>
+        <f t="shared" si="9"/>
         <v>4.333333333333333</v>
       </c>
       <c r="R111" s="3" t="s">
@@ -12936,7 +12942,7 @@
         <v>4</v>
       </c>
       <c r="P112">
-        <f>AVERAGE(J112:O112)</f>
+        <f t="shared" si="9"/>
         <v>4.333333333333333</v>
       </c>
       <c r="R112" s="3" t="s">
@@ -13014,7 +13020,7 @@
         <v>8</v>
       </c>
       <c r="P113">
-        <f>AVERAGE(J113:O113)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="R113" s="3" t="s">
@@ -13092,7 +13098,7 @@
         <v>1</v>
       </c>
       <c r="P114">
-        <f>AVERAGE(J114:O114)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="R114" s="3" t="s">
@@ -13170,7 +13176,7 @@
         <v>4</v>
       </c>
       <c r="P115">
-        <f>AVERAGE(J115:O115)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="R115" s="3" t="s">
@@ -13248,7 +13254,7 @@
         <v>2</v>
       </c>
       <c r="P116">
-        <f>AVERAGE(J116:O116)</f>
+        <f t="shared" si="9"/>
         <v>3.8333333333333335</v>
       </c>
       <c r="R116" s="3" t="s">
@@ -13326,7 +13332,7 @@
         <v>5</v>
       </c>
       <c r="P117">
-        <f>AVERAGE(J117:O117)</f>
+        <f t="shared" si="9"/>
         <v>3.8333333333333335</v>
       </c>
       <c r="R117" s="3" t="s">
@@ -13404,7 +13410,7 @@
         <v>3</v>
       </c>
       <c r="P118">
-        <f>AVERAGE(J118:O118)</f>
+        <f t="shared" si="9"/>
         <v>3.8333333333333335</v>
       </c>
       <c r="R118" s="3" t="s">
@@ -13482,7 +13488,7 @@
         <v>1</v>
       </c>
       <c r="P119">
-        <f>AVERAGE(J119:O119)</f>
+        <f t="shared" si="9"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="R119" s="3" t="s">
@@ -13560,7 +13566,7 @@
         <v>9</v>
       </c>
       <c r="P120">
-        <f>AVERAGE(J120:O120)</f>
+        <f t="shared" si="9"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="R120" s="3" t="s">
@@ -13638,7 +13644,7 @@
         <v>1</v>
       </c>
       <c r="P121">
-        <f>AVERAGE(J121:O121)</f>
+        <f t="shared" si="9"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="R121" s="3" t="s">
@@ -13716,7 +13722,7 @@
         <v>8</v>
       </c>
       <c r="P122">
-        <f>AVERAGE(J122:O122)</f>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="R122" s="3" t="s">
@@ -13794,7 +13800,7 @@
         <v>10</v>
       </c>
       <c r="P123">
-        <f>AVERAGE(J123:O123)</f>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="R123" s="3" t="s">
@@ -13872,7 +13878,7 @@
         <v>1</v>
       </c>
       <c r="P124">
-        <f>AVERAGE(J124:O124)</f>
+        <f t="shared" si="9"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="R124" s="3" t="s">
@@ -13950,7 +13956,7 @@
         <v>6</v>
       </c>
       <c r="P125">
-        <f>AVERAGE(J125:O125)</f>
+        <f t="shared" si="9"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="R125" s="3" t="s">
@@ -14028,7 +14034,7 @@
         <v>2</v>
       </c>
       <c r="P126">
-        <f>AVERAGE(J126:O126)</f>
+        <f t="shared" si="9"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="R126" s="3" t="s">
@@ -14106,7 +14112,7 @@
         <v>3</v>
       </c>
       <c r="P127">
-        <f>AVERAGE(J127:O127)</f>
+        <f t="shared" si="9"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="R127" s="3" t="s">
@@ -14184,7 +14190,7 @@
         <v>5</v>
       </c>
       <c r="P128">
-        <f>AVERAGE(J128:O128)</f>
+        <f t="shared" si="9"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="R128" s="3" t="s">
@@ -14262,7 +14268,7 @@
         <v>5</v>
       </c>
       <c r="P129">
-        <f>AVERAGE(J129:O129)</f>
+        <f t="shared" si="9"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="R129" s="3" t="s">
@@ -14340,7 +14346,7 @@
         <v>1</v>
       </c>
       <c r="P130">
-        <f>AVERAGE(J130:O130)</f>
+        <f t="shared" ref="P130:P161" si="10">AVERAGE(J130:O130)</f>
         <v>3</v>
       </c>
       <c r="R130" s="3" t="s">
@@ -14418,7 +14424,7 @@
         <v>5</v>
       </c>
       <c r="P131">
-        <f>AVERAGE(J131:O131)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R131" s="3" t="s">
@@ -14496,7 +14502,7 @@
         <v>2</v>
       </c>
       <c r="P132">
-        <f>AVERAGE(J132:O132)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R132" s="3" t="s">
@@ -14574,7 +14580,7 @@
         <v>2</v>
       </c>
       <c r="P133">
-        <f>AVERAGE(J133:O133)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R133" s="3" t="s">
@@ -14652,7 +14658,7 @@
         <v>2</v>
       </c>
       <c r="P134">
-        <f>AVERAGE(J134:O134)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R134" s="3" t="s">
@@ -14730,7 +14736,7 @@
         <v>1</v>
       </c>
       <c r="P135">
-        <f>AVERAGE(J135:O135)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R135" s="3" t="s">
@@ -14808,7 +14814,7 @@
         <v>9</v>
       </c>
       <c r="P136">
-        <f>AVERAGE(J136:O136)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R136" s="3" t="s">
@@ -14886,7 +14892,7 @@
         <v>9</v>
       </c>
       <c r="P137">
-        <f>AVERAGE(J137:O137)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R137" s="3" t="s">
@@ -14964,7 +14970,7 @@
         <v>2</v>
       </c>
       <c r="P138">
-        <f>AVERAGE(J138:O138)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R138" s="3" t="s">
@@ -15042,7 +15048,7 @@
         <v>3</v>
       </c>
       <c r="P139">
-        <f>AVERAGE(J139:O139)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R139" s="3" t="s">
@@ -15120,7 +15126,7 @@
         <v>4</v>
       </c>
       <c r="P140">
-        <f>AVERAGE(J140:O140)</f>
+        <f t="shared" si="10"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R140" s="3" t="s">
@@ -15198,7 +15204,7 @@
         <v>6</v>
       </c>
       <c r="P141">
-        <f>AVERAGE(J141:O141)</f>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="R141" s="3" t="s">
@@ -15276,7 +15282,7 @@
         <v>3</v>
       </c>
       <c r="P142">
-        <f>AVERAGE(J142:O142)</f>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="R142" s="3" t="s">
@@ -15354,7 +15360,7 @@
         <v>10</v>
       </c>
       <c r="P143">
-        <f>AVERAGE(J143:O143)</f>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="R143" s="3" t="s">
@@ -15432,7 +15438,7 @@
         <v>6</v>
       </c>
       <c r="P144">
-        <f>AVERAGE(J144:O144)</f>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="R144" s="3" t="s">
@@ -15510,7 +15516,7 @@
         <v>1</v>
       </c>
       <c r="P145">
-        <f>AVERAGE(J145:O145)</f>
+        <f t="shared" si="10"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="R145" s="3" t="s">
@@ -15588,7 +15594,7 @@
         <v>3</v>
       </c>
       <c r="P146">
-        <f>AVERAGE(J146:O146)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R146" s="3" t="s">
@@ -15666,7 +15672,7 @@
         <v>1</v>
       </c>
       <c r="P147">
-        <f>AVERAGE(J147:O147)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R147" s="3" t="s">
@@ -15744,7 +15750,7 @@
         <v>3</v>
       </c>
       <c r="P148">
-        <f>AVERAGE(J148:O148)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R148" s="3" t="s">
@@ -15822,7 +15828,7 @@
         <v>1</v>
       </c>
       <c r="P149">
-        <f>AVERAGE(J149:O149)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R149" s="3" t="s">
@@ -15900,7 +15906,7 @@
         <v>3</v>
       </c>
       <c r="P150">
-        <f>AVERAGE(J150:O150)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R150" s="3" t="s">
@@ -15978,7 +15984,7 @@
         <v>1</v>
       </c>
       <c r="P151">
-        <f>AVERAGE(J151:O151)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R151" s="3" t="s">
@@ -16056,7 +16062,7 @@
         <v>1</v>
       </c>
       <c r="P152">
-        <f>AVERAGE(J152:O152)</f>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="R152" s="3" t="s">
@@ -16134,7 +16140,7 @@
         <v>5</v>
       </c>
       <c r="P153">
-        <f>AVERAGE(J153:O153)</f>
+        <f t="shared" si="10"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="R153" s="3" t="s">
@@ -16212,7 +16218,7 @@
         <v>1</v>
       </c>
       <c r="P154">
-        <f>AVERAGE(J154:O154)</f>
+        <f t="shared" si="10"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="R154" s="3" t="s">
@@ -16290,7 +16296,7 @@
         <v>4</v>
       </c>
       <c r="P155">
-        <f>AVERAGE(J155:O155)</f>
+        <f t="shared" si="10"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="R155" s="3" t="s">
@@ -16368,7 +16374,7 @@
         <v>2</v>
       </c>
       <c r="P156">
-        <f>AVERAGE(J156:O156)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R156" s="3" t="s">
@@ -16446,7 +16452,7 @@
         <v>5</v>
       </c>
       <c r="P157">
-        <f>AVERAGE(J157:O157)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R157" s="3" t="s">
@@ -16524,7 +16530,7 @@
         <v>4</v>
       </c>
       <c r="P158">
-        <f>AVERAGE(J158:O158)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R158" s="3" t="s">
@@ -16602,7 +16608,7 @@
         <v>1</v>
       </c>
       <c r="P159">
-        <f>AVERAGE(J159:O159)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R159" s="3" t="s">
@@ -16680,7 +16686,7 @@
         <v>5</v>
       </c>
       <c r="P160">
-        <f>AVERAGE(J160:O160)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R160" s="3" t="s">
@@ -16758,7 +16764,7 @@
         <v>1</v>
       </c>
       <c r="P161">
-        <f>AVERAGE(J161:O161)</f>
+        <f t="shared" si="10"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R161" s="3" t="s">
@@ -16836,7 +16842,7 @@
         <v>2</v>
       </c>
       <c r="P162">
-        <f>AVERAGE(J162:O162)</f>
+        <f t="shared" ref="P162:P193" si="11">AVERAGE(J162:O162)</f>
         <v>2.1666666666666665</v>
       </c>
       <c r="R162" s="3" t="s">
@@ -16914,7 +16920,7 @@
         <v>1</v>
       </c>
       <c r="P163">
-        <f>AVERAGE(J163:O163)</f>
+        <f t="shared" si="11"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R163" s="3" t="s">
@@ -16992,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="P164">
-        <f>AVERAGE(J164:O164)</f>
+        <f t="shared" si="11"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="R164" s="3" t="s">
@@ -17070,7 +17076,7 @@
         <v>3</v>
       </c>
       <c r="P165">
-        <f>AVERAGE(J165:O165)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R165" s="3" t="s">
@@ -17148,7 +17154,7 @@
         <v>2</v>
       </c>
       <c r="P166">
-        <f>AVERAGE(J166:O166)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R166" s="3" t="s">
@@ -17226,7 +17232,7 @@
         <v>3</v>
       </c>
       <c r="P167">
-        <f>AVERAGE(J167:O167)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R167" s="3" t="s">
@@ -17304,7 +17310,7 @@
         <v>5</v>
       </c>
       <c r="P168">
-        <f>AVERAGE(J168:O168)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R168" s="3" t="s">
@@ -17382,7 +17388,7 @@
         <v>1</v>
       </c>
       <c r="P169">
-        <f>AVERAGE(J169:O169)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R169" s="3" t="s">
@@ -17460,7 +17466,7 @@
         <v>2</v>
       </c>
       <c r="P170">
-        <f>AVERAGE(J170:O170)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R170" s="3" t="s">
@@ -17538,7 +17544,7 @@
         <v>3</v>
       </c>
       <c r="P171">
-        <f>AVERAGE(J171:O171)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R171" s="3" t="s">
@@ -17616,7 +17622,7 @@
         <v>3</v>
       </c>
       <c r="P172">
-        <f>AVERAGE(J172:O172)</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="R172" s="3" t="s">
@@ -17694,7 +17700,7 @@
         <v>2</v>
       </c>
       <c r="P173">
-        <f>AVERAGE(J173:O173)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R173" s="3" t="s">
@@ -17772,7 +17778,7 @@
         <v>2</v>
       </c>
       <c r="P174">
-        <f>AVERAGE(J174:O174)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R174" s="3" t="s">
@@ -17850,7 +17856,7 @@
         <v>1</v>
       </c>
       <c r="P175">
-        <f>AVERAGE(J175:O175)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R175" s="3" t="s">
@@ -17928,7 +17934,7 @@
         <v>3</v>
       </c>
       <c r="P176">
-        <f>AVERAGE(J176:O176)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R176" s="3" t="s">
@@ -18006,7 +18012,7 @@
         <v>3</v>
       </c>
       <c r="P177">
-        <f>AVERAGE(J177:O177)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R177" s="3" t="s">
@@ -18084,7 +18090,7 @@
         <v>4</v>
       </c>
       <c r="P178">
-        <f>AVERAGE(J178:O178)</f>
+        <f t="shared" si="11"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="R178" s="3" t="s">
@@ -18162,7 +18168,7 @@
         <v>2</v>
       </c>
       <c r="P179">
-        <f>AVERAGE(J179:O179)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R179" s="3" t="s">
@@ -18240,7 +18246,7 @@
         <v>2</v>
       </c>
       <c r="P180">
-        <f>AVERAGE(J180:O180)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R180" s="3" t="s">
@@ -18318,7 +18324,7 @@
         <v>3</v>
       </c>
       <c r="P181">
-        <f>AVERAGE(J181:O181)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R181" s="3" t="s">
@@ -18396,7 +18402,7 @@
         <v>1</v>
       </c>
       <c r="P182">
-        <f>AVERAGE(J182:O182)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R182" s="3" t="s">
@@ -18474,7 +18480,7 @@
         <v>1</v>
       </c>
       <c r="P183">
-        <f>AVERAGE(J183:O183)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R183" s="3" t="s">
@@ -18552,7 +18558,7 @@
         <v>3</v>
       </c>
       <c r="P184">
-        <f>AVERAGE(J184:O184)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R184" s="3" t="s">
@@ -18630,7 +18636,7 @@
         <v>2</v>
       </c>
       <c r="P185">
-        <f>AVERAGE(J185:O185)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R185" s="3" t="s">
@@ -18708,7 +18714,7 @@
         <v>3</v>
       </c>
       <c r="P186">
-        <f>AVERAGE(J186:O186)</f>
+        <f t="shared" si="11"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="R186" s="3" t="s">
@@ -18786,7 +18792,7 @@
         <v>2</v>
       </c>
       <c r="P187">
-        <f>AVERAGE(J187:O187)</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="R187" s="3" t="s">
@@ -18864,7 +18870,7 @@
         <v>1</v>
       </c>
       <c r="P188">
-        <f>AVERAGE(J188:O188)</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="R188" s="3" t="s">
@@ -18942,7 +18948,7 @@
         <v>2</v>
       </c>
       <c r="P189">
-        <f>AVERAGE(J189:O189)</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="R189" s="3" t="s">
@@ -19020,7 +19026,7 @@
         <v>1</v>
       </c>
       <c r="P190">
-        <f>AVERAGE(J190:O190)</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="R190" s="3" t="s">
@@ -19098,7 +19104,7 @@
         <v>3</v>
       </c>
       <c r="P191">
-        <f>AVERAGE(J191:O191)</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
       <c r="R191" s="3" t="s">
@@ -19176,7 +19182,7 @@
         <v>1</v>
       </c>
       <c r="P192">
-        <f>AVERAGE(J192:O192)</f>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="R192" s="3" t="s">
@@ -19254,7 +19260,7 @@
         <v>1</v>
       </c>
       <c r="P193">
-        <f>AVERAGE(J193:O193)</f>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="R193" s="3" t="s">
@@ -19332,7 +19338,7 @@
         <v>1</v>
       </c>
       <c r="P194">
-        <f>AVERAGE(J194:O194)</f>
+        <f t="shared" ref="P194:P225" si="12">AVERAGE(J194:O194)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="R194" s="3" t="s">
@@ -19373,7 +19379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC91AE-BB3C-D445-857D-BF013CB9D47D}">
   <dimension ref="A1:AA1096"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="O27" sqref="O27:O28"/>
     </sheetView>
   </sheetViews>
@@ -21827,7 +21833,7 @@
       <c r="M27" s="6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="8" t="s">
         <v>515</v>
       </c>
       <c r="P27" s="6" t="str">
@@ -21919,7 +21925,7 @@
       <c r="M28" s="6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="O28" s="8" t="s">
         <v>616</v>
       </c>
       <c r="P28" s="6" t="str">
@@ -33511,7 +33517,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="H1:I28"/>
+      <selection activeCell="D27" sqref="D27:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34075,6 +34081,13 @@
       <c r="B27" t="s">
         <v>840</v>
       </c>
+      <c r="D27" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" ref="E27:E28" si="1">VLOOKUP($D27,$A$1:$B$194,2,FALSE)</f>
+        <v>Faecalibacterium prausnitzii</v>
+      </c>
       <c r="H27" t="s">
         <v>856</v>
       </c>
@@ -34088,6 +34101,13 @@
       </c>
       <c r="B28" t="s">
         <v>827</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>Caudovirales sp.</v>
       </c>
       <c r="H28" t="s">
         <v>878</v>
@@ -40106,8 +40126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7192636B-1268-864E-BFD4-8694A9B5E7B9}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41477,14 +41497,174 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4111CD-3CDF-CF4B-987C-2E286C9BEC80}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>881</v>
+      </c>
+      <c r="B2" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>880</v>
+      </c>
+      <c r="B3" t="s">
+        <v>834</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E6">
+        <v>0.65795499999999996</v>
+      </c>
+      <c r="F6">
+        <v>0.66333299999999995</v>
+      </c>
+      <c r="G6">
+        <v>0.66333299999999995</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E7">
+        <v>0.33201000000000003</v>
+      </c>
+      <c r="F7">
+        <v>0.3725</v>
+      </c>
+      <c r="G7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -41494,7 +41674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAAE699E-7123-764F-9D7E-BD7665879B91}">
   <dimension ref="A1:H421"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+    <sheetView zoomScale="157" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to genomic context info
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC832F57-3522-0D48-8632-3A8AF2E06B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263CB06F-CEEA-5D44-85CB-C5DCB1D61439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="883">
   <si>
     <t>Seq ID</t>
   </si>
@@ -2688,6 +2688,9 @@
   </si>
   <si>
     <t>AMP_144878_c1_g1_i1.p9</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -19338,7 +19341,7 @@
         <v>1</v>
       </c>
       <c r="P194">
-        <f t="shared" ref="P194:P225" si="12">AVERAGE(J194:O194)</f>
+        <f t="shared" ref="P194" si="12">AVERAGE(J194:O194)</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="R194" s="3" t="s">
@@ -19379,8 +19382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC91AE-BB3C-D445-857D-BF013CB9D47D}">
   <dimension ref="A1:AA1096"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27:O28"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33517,7 +33520,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:E28"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34043,7 +34046,7 @@
         <v>370</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
+        <f>VLOOKUP($D25,$A$1:$B$194,2,FALSE)</f>
         <v>Myoviridae sp.</v>
       </c>
       <c r="H25" t="s">
@@ -40126,8 +40129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7192636B-1268-864E-BFD4-8694A9B5E7B9}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" activeCellId="1" sqref="A13 C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40137,7 +40140,7 @@
     <col min="3" max="3" width="82.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>747</v>
       </c>
@@ -40148,18 +40151,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>724</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>361</v>
       </c>
@@ -40170,18 +40173,18 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>498</v>
       </c>
@@ -40192,7 +40195,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>424</v>
       </c>
@@ -40203,7 +40206,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>627</v>
       </c>
@@ -40214,7 +40217,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>409</v>
       </c>
@@ -40225,7 +40228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>546</v>
       </c>
@@ -40236,18 +40239,21 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>762</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>527</v>
       </c>
@@ -40258,7 +40264,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>395</v>
       </c>
@@ -40269,7 +40275,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>435</v>
       </c>
@@ -40280,7 +40286,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>513</v>
       </c>
@@ -40291,7 +40297,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>607</v>
       </c>
@@ -40302,7 +40308,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>562</v>
       </c>
@@ -40317,10 +40323,10 @@
       <c r="A17" s="14" t="s">
         <v>668</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>174</v>
       </c>
     </row>
@@ -40372,21 +40378,24 @@
       <c r="A22" s="14" t="s">
         <v>584</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>325</v>
+      </c>
+      <c r="D22" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>655</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>267</v>
       </c>
     </row>
@@ -40394,10 +40403,10 @@
       <c r="A24" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>225</v>
       </c>
     </row>
@@ -40416,10 +40425,10 @@
       <c r="A26" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>838</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>132</v>
       </c>
     </row>
@@ -41499,7 +41508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4111CD-3CDF-CF4B-987C-2E286C9BEC80}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Gravy and net charge analysis added
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263CB06F-CEEA-5D44-85CB-C5DCB1D61439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95C10BF-F0C4-424F-B792-83E4AC33503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="amps_overexpressed_info" sheetId="4" r:id="rId5"/>
     <sheet name="amps_allsamples_info" sheetId="5" r:id="rId6"/>
     <sheet name="workbench_blastn" sheetId="9" r:id="rId7"/>
+    <sheet name="tmp" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="913">
   <si>
     <t>Seq ID</t>
   </si>
@@ -2691,6 +2692,96 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>GRAVY index</t>
+  </si>
+  <si>
+    <t>Net charge at pH 7</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN138200_c2_g1_i1.p2</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN141075_c3_g1_i1.p9</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN143020_c3_g1_i1.p2</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN143683_c0_g2_i1.p14</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN144897_c3_g1_i5.p10</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN385865_c1_g1_i1.p3</t>
+  </si>
+  <si>
+    <t>Ob</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN125192_c2_g1_i1.p8</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN133076_c0_g4_i1.p5</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN138681_c7_g1_i1.p3</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN142115_c6_g1_i3.p7</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN142526_c5_g1_i7.p5</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN142823_c1_g1_i2.p2</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN143096_c2_g1_i1.p6</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN144187_c0_g1_i10.p9</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN144483_c7_g1_i1.p5</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN144624_c4_g1_i1.p5</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN144653_c7_g8_i1.p24</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN145055_c3_g1_i3.p7</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN145062_c3_g1_i3.p10</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN145245_c6_g1_i2.p2</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN145391_c5_g1_i9.p5</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN145575_c0_g1_i3.p4</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN612198_c2_g1_i1.p1</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN7230_c1_g2_i2.p9</t>
+  </si>
+  <si>
+    <t>&gt;TRINITY_DN851511_c0_g1_i1.p12</t>
+  </si>
+  <si>
+    <t>OMS</t>
   </si>
 </sst>
 </file>
@@ -33584,7 +33675,7 @@
         <v>361</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E25" si="0">VLOOKUP($D3,$A$1:$B$194,2,FALSE)</f>
+        <f t="shared" ref="E3:E24" si="0">VLOOKUP($D3,$A$1:$B$194,2,FALSE)</f>
         <v>Siphoviridae sp.</v>
       </c>
       <c r="H3" t="s">
@@ -40130,7 +40221,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" activeCellId="1" sqref="A13 C30"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48076,4 +48167,724 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EF931D-DD83-C94C-8019-1057FD3D9B20}">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="A1:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B2" t="s">
+        <v>892</v>
+      </c>
+      <c r="C2">
+        <v>-0.41388888888888797</v>
+      </c>
+      <c r="D2">
+        <v>6.4714511567774098</v>
+      </c>
+      <c r="G2" t="s">
+        <v>873</v>
+      </c>
+      <c r="H2" t="s">
+        <v>884</v>
+      </c>
+      <c r="I2" t="s">
+        <v>873</v>
+      </c>
+      <c r="J2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>892</v>
+      </c>
+      <c r="C3">
+        <v>-1.69999999999999</v>
+      </c>
+      <c r="D3">
+        <v>3.4579619161958002</v>
+      </c>
+      <c r="G3" t="s">
+        <v>886</v>
+      </c>
+      <c r="H3">
+        <v>-0.41388888888888797</v>
+      </c>
+      <c r="I3" t="s">
+        <v>785</v>
+      </c>
+      <c r="J3">
+        <v>6.4714511567774098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>892</v>
+      </c>
+      <c r="C4">
+        <v>0.149999999999999</v>
+      </c>
+      <c r="D4">
+        <v>3.7611275943461902</v>
+      </c>
+      <c r="G4" t="s">
+        <v>887</v>
+      </c>
+      <c r="H4">
+        <v>-1.69999999999999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4">
+        <v>3.4579619161958002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C5">
+        <v>-1.6666666666666701E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.49935568654234302</v>
+      </c>
+      <c r="G5" t="s">
+        <v>888</v>
+      </c>
+      <c r="H5">
+        <v>0.149999999999999</v>
+      </c>
+      <c r="I5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5">
+        <v>3.7611275943461902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>892</v>
+      </c>
+      <c r="C6">
+        <v>-1.7222222222222201</v>
+      </c>
+      <c r="D6">
+        <v>1.5011571476165499</v>
+      </c>
+      <c r="G6" t="s">
+        <v>889</v>
+      </c>
+      <c r="H6">
+        <v>-1.6666666666666701E-2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6">
+        <v>0.49935568654234302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>892</v>
+      </c>
+      <c r="C7">
+        <v>-0.79199999999999904</v>
+      </c>
+      <c r="D7">
+        <v>0.76313559624419802</v>
+      </c>
+      <c r="G7" t="s">
+        <v>890</v>
+      </c>
+      <c r="H7">
+        <v>-1.7222222222222201</v>
+      </c>
+      <c r="I7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J7">
+        <v>1.5011571476165499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>912</v>
+      </c>
+      <c r="C8">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="D8">
+        <v>1.49934568664234</v>
+      </c>
+      <c r="G8" t="s">
+        <v>891</v>
+      </c>
+      <c r="H8">
+        <v>-0.79199999999999904</v>
+      </c>
+      <c r="I8" t="s">
+        <v>310</v>
+      </c>
+      <c r="J8">
+        <v>0.76313559624419802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>912</v>
+      </c>
+      <c r="C9">
+        <v>-0.82307692307692304</v>
+      </c>
+      <c r="D9">
+        <v>-0.32226295389458598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>912</v>
+      </c>
+      <c r="C10">
+        <v>-0.75151515151515103</v>
+      </c>
+      <c r="D10">
+        <v>6.7489650825674898</v>
+      </c>
+      <c r="G10" t="s">
+        <v>873</v>
+      </c>
+      <c r="H10" t="s">
+        <v>884</v>
+      </c>
+      <c r="I10" t="s">
+        <v>873</v>
+      </c>
+      <c r="J10" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>912</v>
+      </c>
+      <c r="C11">
+        <v>-0.44444444444444398</v>
+      </c>
+      <c r="D11">
+        <v>-0.499523552517811</v>
+      </c>
+      <c r="G11" t="s">
+        <v>893</v>
+      </c>
+      <c r="H11">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>1.49934568664234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>912</v>
+      </c>
+      <c r="C12">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="D12">
+        <v>1.7561056101932899</v>
+      </c>
+      <c r="G12" t="s">
+        <v>894</v>
+      </c>
+      <c r="H12">
+        <v>-0.82307692307692304</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>-0.32226295389458598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>798</v>
+      </c>
+      <c r="B13" t="s">
+        <v>912</v>
+      </c>
+      <c r="C13">
+        <v>-0.32380952380952299</v>
+      </c>
+      <c r="D13">
+        <v>1.9260375560165699</v>
+      </c>
+      <c r="G13" t="s">
+        <v>895</v>
+      </c>
+      <c r="H13">
+        <v>-0.75151515151515103</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13">
+        <v>6.7489650825674898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>912</v>
+      </c>
+      <c r="C14">
+        <v>-1.5538461538461501</v>
+      </c>
+      <c r="D14">
+        <v>5.7530986072962902</v>
+      </c>
+      <c r="G14" t="s">
+        <v>896</v>
+      </c>
+      <c r="H14">
+        <v>-0.44444444444444398</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14">
+        <v>-0.499523552517811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" t="s">
+        <v>912</v>
+      </c>
+      <c r="C15">
+        <v>-3.3571428571428501</v>
+      </c>
+      <c r="D15">
+        <v>0.76003683310635395</v>
+      </c>
+      <c r="G15" t="s">
+        <v>897</v>
+      </c>
+      <c r="H15">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15">
+        <v>1.7561056101932899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" t="s">
+        <v>912</v>
+      </c>
+      <c r="C16">
+        <v>0.628571428571428</v>
+      </c>
+      <c r="D16">
+        <v>-0.32729493794748299</v>
+      </c>
+      <c r="G16" t="s">
+        <v>898</v>
+      </c>
+      <c r="H16">
+        <v>-0.32380952380952299</v>
+      </c>
+      <c r="I16" t="s">
+        <v>798</v>
+      </c>
+      <c r="J16">
+        <v>1.9260375560165699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" t="s">
+        <v>912</v>
+      </c>
+      <c r="C17">
+        <v>0.55714285714285705</v>
+      </c>
+      <c r="D17">
+        <v>1.49934568664234</v>
+      </c>
+      <c r="G17" t="s">
+        <v>899</v>
+      </c>
+      <c r="H17">
+        <v>-1.5538461538461501</v>
+      </c>
+      <c r="I17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17">
+        <v>5.7530986072962902</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" t="s">
+        <v>912</v>
+      </c>
+      <c r="C18">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D18">
+        <v>-4.4858548868306896</v>
+      </c>
+      <c r="G18" t="s">
+        <v>900</v>
+      </c>
+      <c r="H18">
+        <v>-3.3571428571428501</v>
+      </c>
+      <c r="I18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18">
+        <v>0.76003683310635395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" t="s">
+        <v>912</v>
+      </c>
+      <c r="C19">
+        <v>1.99999999999999E-2</v>
+      </c>
+      <c r="D19">
+        <v>-0.499523552517811</v>
+      </c>
+      <c r="G19" t="s">
+        <v>901</v>
+      </c>
+      <c r="H19">
+        <v>0.628571428571428</v>
+      </c>
+      <c r="I19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19">
+        <v>-0.32729493794748299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" t="s">
+        <v>912</v>
+      </c>
+      <c r="C20">
+        <v>-3.73999999999999</v>
+      </c>
+      <c r="D20">
+        <v>1.83383061570099</v>
+      </c>
+      <c r="G20" t="s">
+        <v>902</v>
+      </c>
+      <c r="H20">
+        <v>0.55714285714285705</v>
+      </c>
+      <c r="I20" t="s">
+        <v>184</v>
+      </c>
+      <c r="J20">
+        <v>1.49934568664234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" t="s">
+        <v>912</v>
+      </c>
+      <c r="C21">
+        <v>-1.0344827586206799E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.7584488922138199</v>
+      </c>
+      <c r="G21" t="s">
+        <v>903</v>
+      </c>
+      <c r="H21">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="I21" t="s">
+        <v>190</v>
+      </c>
+      <c r="J21">
+        <v>-4.4858548868306896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" t="s">
+        <v>912</v>
+      </c>
+      <c r="C22">
+        <v>-2.57777777777777</v>
+      </c>
+      <c r="D22">
+        <v>0.50396760958976194</v>
+      </c>
+      <c r="G22" t="s">
+        <v>904</v>
+      </c>
+      <c r="H22">
+        <v>1.99999999999999E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>224</v>
+      </c>
+      <c r="J22">
+        <v>-0.499523552517811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" t="s">
+        <v>912</v>
+      </c>
+      <c r="C23">
+        <v>-1.67777777777777</v>
+      </c>
+      <c r="D23">
+        <v>0.50215614861555302</v>
+      </c>
+      <c r="G23" t="s">
+        <v>905</v>
+      </c>
+      <c r="H23">
+        <v>-3.73999999999999</v>
+      </c>
+      <c r="I23" t="s">
+        <v>226</v>
+      </c>
+      <c r="J23">
+        <v>1.83383061570099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B24" t="s">
+        <v>912</v>
+      </c>
+      <c r="C24">
+        <v>-1.5414634146341399</v>
+      </c>
+      <c r="D24">
+        <v>3.9380451106218302</v>
+      </c>
+      <c r="G24" t="s">
+        <v>906</v>
+      </c>
+      <c r="H24">
+        <v>-1.0344827586206799E-2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>233</v>
+      </c>
+      <c r="J24">
+        <v>1.7584488922138199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>322</v>
+      </c>
+      <c r="B25" t="s">
+        <v>912</v>
+      </c>
+      <c r="C25">
+        <v>-1.0625</v>
+      </c>
+      <c r="D25">
+        <v>0.50297860849076204</v>
+      </c>
+      <c r="G25" t="s">
+        <v>907</v>
+      </c>
+      <c r="H25">
+        <v>-2.57777777777777</v>
+      </c>
+      <c r="I25" t="s">
+        <v>268</v>
+      </c>
+      <c r="J25">
+        <v>0.50396760958976194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" t="s">
+        <v>912</v>
+      </c>
+      <c r="C26">
+        <v>1.3285714285714201</v>
+      </c>
+      <c r="D26">
+        <v>-0.49964531245865501</v>
+      </c>
+      <c r="G26" t="s">
+        <v>908</v>
+      </c>
+      <c r="H26">
+        <v>-1.67777777777777</v>
+      </c>
+      <c r="I26" t="s">
+        <v>286</v>
+      </c>
+      <c r="J26">
+        <v>0.50215614861555302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>909</v>
+      </c>
+      <c r="H27">
+        <v>-1.5414634146341399</v>
+      </c>
+      <c r="I27" t="s">
+        <v>316</v>
+      </c>
+      <c r="J27">
+        <v>3.9380451106218302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>910</v>
+      </c>
+      <c r="H28">
+        <v>-1.0625</v>
+      </c>
+      <c r="I28" t="s">
+        <v>322</v>
+      </c>
+      <c r="J28">
+        <v>0.50297860849076204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>911</v>
+      </c>
+      <c r="H29">
+        <v>1.3285714285714201</v>
+      </c>
+      <c r="I29" t="s">
+        <v>324</v>
+      </c>
+      <c r="J29">
+        <v>-0.49964531245865501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creation of overexpressed boxplots
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95C10BF-F0C4-424F-B792-83E4AC33503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B4A7AA-645D-4543-B092-8921F45EEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="7" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3708" uniqueCount="888">
   <si>
     <t>Seq ID</t>
   </si>
@@ -2697,91 +2697,16 @@
     <t>group</t>
   </si>
   <si>
-    <t>GRAVY index</t>
-  </si>
-  <si>
-    <t>Net charge at pH 7</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN138200_c2_g1_i1.p2</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN141075_c3_g1_i1.p9</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN143020_c3_g1_i1.p2</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN143683_c0_g2_i1.p14</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN144897_c3_g1_i5.p10</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN385865_c1_g1_i1.p3</t>
-  </si>
-  <si>
     <t>Ob</t>
   </si>
   <si>
-    <t>&gt;TRINITY_DN125192_c2_g1_i1.p8</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN133076_c0_g4_i1.p5</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN138681_c7_g1_i1.p3</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN142115_c6_g1_i3.p7</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN142526_c5_g1_i7.p5</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN142823_c1_g1_i2.p2</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN143096_c2_g1_i1.p6</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN144187_c0_g1_i10.p9</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN144483_c7_g1_i1.p5</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN144624_c4_g1_i1.p5</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN144653_c7_g8_i1.p24</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN145055_c3_g1_i3.p7</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN145062_c3_g1_i3.p10</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN145245_c6_g1_i2.p2</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN145391_c5_g1_i9.p5</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN145575_c0_g1_i3.p4</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN612198_c2_g1_i1.p1</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN7230_c1_g2_i2.p9</t>
-  </si>
-  <si>
-    <t>&gt;TRINITY_DN851511_c0_g1_i1.p12</t>
-  </si>
-  <si>
     <t>OMS</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>number_AMPs</t>
   </si>
 </sst>
 </file>
@@ -40220,8 +40145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7192636B-1268-864E-BFD4-8694A9B5E7B9}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48171,719 +48096,374 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EF931D-DD83-C94C-8019-1057FD3D9B20}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>873</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>724</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="D1" t="s">
+        <v>886</v>
+      </c>
+      <c r="E1" t="s">
         <v>883</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" t="s">
+        <v>833</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="E2" t="s">
         <v>884</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="D3" t="s">
+        <v>849</v>
+      </c>
+      <c r="E3" t="s">
+        <v>884</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="B4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="E4" t="s">
+        <v>884</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" t="s">
+        <v>849</v>
+      </c>
+      <c r="D5" t="s">
+        <v>833</v>
+      </c>
+      <c r="E5" t="s">
+        <v>884</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="B6" t="s">
+        <v>827</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="E6" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>785</v>
-      </c>
-      <c r="B2" t="s">
-        <v>892</v>
-      </c>
-      <c r="C2">
-        <v>-0.41388888888888797</v>
-      </c>
-      <c r="D2">
-        <v>6.4714511567774098</v>
-      </c>
-      <c r="G2" t="s">
-        <v>873</v>
-      </c>
-      <c r="H2" t="s">
-        <v>884</v>
-      </c>
-      <c r="I2" t="s">
-        <v>873</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="B7" t="s">
+        <v>850</v>
+      </c>
+      <c r="D7" t="s">
+        <v>840</v>
+      </c>
+      <c r="E7" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" t="s">
-        <v>892</v>
-      </c>
-      <c r="C3">
-        <v>-1.69999999999999</v>
-      </c>
-      <c r="D3">
-        <v>3.4579619161958002</v>
-      </c>
-      <c r="G3" t="s">
-        <v>886</v>
-      </c>
-      <c r="H3">
-        <v>-0.41388888888888797</v>
-      </c>
-      <c r="I3" t="s">
-        <v>785</v>
-      </c>
-      <c r="J3">
-        <v>6.4714511567774098</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>892</v>
-      </c>
-      <c r="C4">
-        <v>0.149999999999999</v>
-      </c>
-      <c r="D4">
-        <v>3.7611275943461902</v>
-      </c>
-      <c r="G4" t="s">
-        <v>887</v>
-      </c>
-      <c r="H4">
-        <v>-1.69999999999999</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4">
-        <v>3.4579619161958002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" t="s">
-        <v>892</v>
-      </c>
-      <c r="C5">
-        <v>-1.6666666666666701E-2</v>
-      </c>
-      <c r="D5">
-        <v>0.49935568654234302</v>
-      </c>
-      <c r="G5" t="s">
-        <v>888</v>
-      </c>
-      <c r="H5">
-        <v>0.149999999999999</v>
-      </c>
-      <c r="I5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J5">
-        <v>3.7611275943461902</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" t="s">
-        <v>892</v>
-      </c>
-      <c r="C6">
-        <v>-1.7222222222222201</v>
-      </c>
-      <c r="D6">
-        <v>1.5011571476165499</v>
-      </c>
-      <c r="G6" t="s">
-        <v>889</v>
-      </c>
-      <c r="H6">
-        <v>-1.6666666666666701E-2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6">
-        <v>0.49935568654234302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" t="s">
-        <v>892</v>
-      </c>
-      <c r="C7">
-        <v>-0.79199999999999904</v>
-      </c>
-      <c r="D7">
-        <v>0.76313559624419802</v>
-      </c>
-      <c r="G7" t="s">
-        <v>890</v>
-      </c>
-      <c r="H7">
-        <v>-1.7222222222222201</v>
-      </c>
-      <c r="I7" t="s">
-        <v>214</v>
-      </c>
-      <c r="J7">
-        <v>1.5011571476165499</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>546</v>
       </c>
       <c r="B8" t="s">
-        <v>912</v>
-      </c>
-      <c r="C8">
-        <v>0.27777777777777701</v>
-      </c>
-      <c r="D8">
-        <v>1.49934568664234</v>
-      </c>
-      <c r="G8" t="s">
-        <v>891</v>
-      </c>
-      <c r="H8">
-        <v>-0.79199999999999904</v>
-      </c>
-      <c r="I8" t="s">
-        <v>310</v>
-      </c>
-      <c r="J8">
-        <v>0.76313559624419802</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>912</v>
-      </c>
-      <c r="C9">
-        <v>-0.82307692307692304</v>
-      </c>
-      <c r="D9">
-        <v>-0.32226295389458598</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>68</v>
+        <v>827</v>
+      </c>
+      <c r="D8" t="s">
+        <v>833</v>
+      </c>
+      <c r="E8" t="s">
+        <v>885</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>762</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="E9" t="s">
+        <v>885</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>527</v>
       </c>
       <c r="B10" t="s">
-        <v>912</v>
-      </c>
-      <c r="C10">
-        <v>-0.75151515151515103</v>
-      </c>
-      <c r="D10">
-        <v>6.7489650825674898</v>
-      </c>
-      <c r="G10" t="s">
-        <v>873</v>
-      </c>
-      <c r="H10" t="s">
-        <v>884</v>
-      </c>
-      <c r="I10" t="s">
-        <v>873</v>
-      </c>
-      <c r="J10" t="s">
+        <v>853</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="E10" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>94</v>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>395</v>
       </c>
       <c r="B11" t="s">
-        <v>912</v>
-      </c>
-      <c r="C11">
-        <v>-0.44444444444444398</v>
-      </c>
-      <c r="D11">
-        <v>-0.499523552517811</v>
-      </c>
-      <c r="G11" t="s">
-        <v>893</v>
-      </c>
-      <c r="H11">
-        <v>0.27777777777777701</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>1.49934568664234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>110</v>
+        <v>840</v>
+      </c>
+      <c r="D11" t="s">
+        <v>850</v>
+      </c>
+      <c r="E11" t="s">
+        <v>885</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>435</v>
       </c>
       <c r="B12" t="s">
-        <v>912</v>
-      </c>
-      <c r="C12">
-        <v>0.39999999999999902</v>
-      </c>
-      <c r="D12">
-        <v>1.7561056101932899</v>
-      </c>
-      <c r="G12" t="s">
-        <v>894</v>
-      </c>
-      <c r="H12">
-        <v>-0.82307692307692304</v>
-      </c>
-      <c r="I12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12">
-        <v>-0.32226295389458598</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>798</v>
+        <v>831</v>
+      </c>
+      <c r="D12" t="s">
+        <v>832</v>
+      </c>
+      <c r="E12" t="s">
+        <v>885</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>513</v>
       </c>
       <c r="B13" t="s">
-        <v>912</v>
-      </c>
-      <c r="C13">
-        <v>-0.32380952380952299</v>
-      </c>
-      <c r="D13">
-        <v>1.9260375560165699</v>
-      </c>
-      <c r="G13" t="s">
-        <v>895</v>
-      </c>
-      <c r="H13">
-        <v>-0.75151515151515103</v>
-      </c>
-      <c r="I13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13">
-        <v>6.7489650825674898</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>131</v>
+        <v>840</v>
+      </c>
+      <c r="D13" t="s">
+        <v>827</v>
+      </c>
+      <c r="E13" t="s">
+        <v>885</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>607</v>
       </c>
       <c r="B14" t="s">
-        <v>912</v>
-      </c>
-      <c r="C14">
-        <v>-1.5538461538461501</v>
-      </c>
-      <c r="D14">
-        <v>5.7530986072962902</v>
-      </c>
-      <c r="G14" t="s">
-        <v>896</v>
-      </c>
-      <c r="H14">
-        <v>-0.44444444444444398</v>
-      </c>
-      <c r="I14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14">
-        <v>-0.499523552517811</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>157</v>
+        <v>827</v>
+      </c>
+      <c r="D14" t="s">
+        <v>822</v>
+      </c>
+      <c r="E14" t="s">
+        <v>885</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>562</v>
       </c>
       <c r="B15" t="s">
-        <v>912</v>
-      </c>
-      <c r="C15">
-        <v>-3.3571428571428501</v>
-      </c>
-      <c r="D15">
-        <v>0.76003683310635395</v>
-      </c>
-      <c r="G15" t="s">
-        <v>897</v>
-      </c>
-      <c r="H15">
-        <v>0.39999999999999902</v>
-      </c>
-      <c r="I15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J15">
-        <v>1.7561056101932899</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" t="s">
-        <v>912</v>
-      </c>
-      <c r="C16">
-        <v>0.628571428571428</v>
-      </c>
-      <c r="D16">
-        <v>-0.32729493794748299</v>
-      </c>
-      <c r="G16" t="s">
-        <v>898</v>
-      </c>
-      <c r="H16">
-        <v>-0.32380952380952299</v>
-      </c>
-      <c r="I16" t="s">
-        <v>798</v>
-      </c>
-      <c r="J16">
-        <v>1.9260375560165699</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>184</v>
+        <v>822</v>
+      </c>
+      <c r="D15" t="s">
+        <v>835</v>
+      </c>
+      <c r="E15" t="s">
+        <v>885</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="D16" t="s">
+        <v>853</v>
+      </c>
+      <c r="E16" t="s">
+        <v>885</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>638</v>
       </c>
       <c r="B17" t="s">
-        <v>912</v>
-      </c>
-      <c r="C17">
-        <v>0.55714285714285705</v>
-      </c>
-      <c r="D17">
-        <v>1.49934568664234</v>
-      </c>
-      <c r="G17" t="s">
-        <v>899</v>
-      </c>
-      <c r="H17">
-        <v>-1.5538461538461501</v>
-      </c>
-      <c r="I17" t="s">
-        <v>131</v>
-      </c>
-      <c r="J17">
-        <v>5.7530986072962902</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>190</v>
+        <v>835</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>352</v>
       </c>
       <c r="B18" t="s">
-        <v>912</v>
-      </c>
-      <c r="C18">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="D18">
-        <v>-4.4858548868306896</v>
-      </c>
-      <c r="G18" t="s">
-        <v>900</v>
-      </c>
-      <c r="H18">
-        <v>-3.3571428571428501</v>
-      </c>
-      <c r="I18" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18">
-        <v>0.76003683310635395</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>224</v>
+        <v>827</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="B19" t="s">
-        <v>912</v>
-      </c>
-      <c r="C19">
-        <v>1.99999999999999E-2</v>
-      </c>
-      <c r="D19">
-        <v>-0.499523552517811</v>
-      </c>
-      <c r="G19" t="s">
-        <v>901</v>
-      </c>
-      <c r="H19">
-        <v>0.628571428571428</v>
-      </c>
-      <c r="I19" t="s">
-        <v>173</v>
-      </c>
-      <c r="J19">
-        <v>-0.32729493794748299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>226</v>
+        <v>833</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>346</v>
       </c>
       <c r="B20" t="s">
-        <v>912</v>
-      </c>
-      <c r="C20">
-        <v>-3.73999999999999</v>
-      </c>
-      <c r="D20">
-        <v>1.83383061570099</v>
-      </c>
-      <c r="G20" t="s">
-        <v>902</v>
-      </c>
-      <c r="H20">
-        <v>0.55714285714285705</v>
-      </c>
-      <c r="I20" t="s">
-        <v>184</v>
-      </c>
-      <c r="J20">
-        <v>1.49934568664234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" t="s">
-        <v>912</v>
-      </c>
-      <c r="C21">
-        <v>-1.0344827586206799E-2</v>
-      </c>
-      <c r="D21">
-        <v>1.7584488922138199</v>
-      </c>
-      <c r="G21" t="s">
-        <v>903</v>
-      </c>
-      <c r="H21">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="I21" t="s">
-        <v>190</v>
-      </c>
-      <c r="J21">
-        <v>-4.4858548868306896</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" t="s">
-        <v>912</v>
-      </c>
-      <c r="C22">
-        <v>-2.57777777777777</v>
-      </c>
-      <c r="D22">
-        <v>0.50396760958976194</v>
-      </c>
-      <c r="G22" t="s">
-        <v>904</v>
-      </c>
-      <c r="H22">
-        <v>1.99999999999999E-2</v>
-      </c>
-      <c r="I22" t="s">
-        <v>224</v>
-      </c>
-      <c r="J22">
-        <v>-0.499523552517811</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>286</v>
-      </c>
-      <c r="B23" t="s">
-        <v>912</v>
-      </c>
-      <c r="C23">
-        <v>-1.67777777777777</v>
-      </c>
-      <c r="D23">
-        <v>0.50215614861555302</v>
-      </c>
-      <c r="G23" t="s">
-        <v>905</v>
-      </c>
-      <c r="H23">
-        <v>-3.73999999999999</v>
-      </c>
-      <c r="I23" t="s">
-        <v>226</v>
-      </c>
-      <c r="J23">
-        <v>1.83383061570099</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>316</v>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>534</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>370</v>
       </c>
       <c r="B24" t="s">
-        <v>912</v>
-      </c>
-      <c r="C24">
-        <v>-1.5414634146341399</v>
-      </c>
-      <c r="D24">
-        <v>3.9380451106218302</v>
-      </c>
-      <c r="G24" t="s">
-        <v>906</v>
-      </c>
-      <c r="H24">
-        <v>-1.0344827586206799E-2</v>
-      </c>
-      <c r="I24" t="s">
-        <v>233</v>
-      </c>
-      <c r="J24">
-        <v>1.7584488922138199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>322</v>
-      </c>
-      <c r="B25" t="s">
-        <v>912</v>
-      </c>
-      <c r="C25">
-        <v>-1.0625</v>
-      </c>
-      <c r="D25">
-        <v>0.50297860849076204</v>
-      </c>
-      <c r="G25" t="s">
-        <v>907</v>
-      </c>
-      <c r="H25">
-        <v>-2.57777777777777</v>
-      </c>
-      <c r="I25" t="s">
-        <v>268</v>
-      </c>
-      <c r="J25">
-        <v>0.50396760958976194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>324</v>
-      </c>
-      <c r="B26" t="s">
-        <v>912</v>
-      </c>
-      <c r="C26">
-        <v>1.3285714285714201</v>
-      </c>
-      <c r="D26">
-        <v>-0.49964531245865501</v>
-      </c>
-      <c r="G26" t="s">
-        <v>908</v>
-      </c>
-      <c r="H26">
-        <v>-1.67777777777777</v>
-      </c>
-      <c r="I26" t="s">
-        <v>286</v>
-      </c>
-      <c r="J26">
-        <v>0.50215614861555302</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
-        <v>909</v>
-      </c>
-      <c r="H27">
-        <v>-1.5414634146341399</v>
-      </c>
-      <c r="I27" t="s">
-        <v>316</v>
-      </c>
-      <c r="J27">
-        <v>3.9380451106218302</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
-        <v>910</v>
-      </c>
-      <c r="H28">
-        <v>-1.0625</v>
-      </c>
-      <c r="I28" t="s">
-        <v>322</v>
-      </c>
-      <c r="J28">
-        <v>0.50297860849076204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G29" t="s">
-        <v>911</v>
-      </c>
-      <c r="H29">
-        <v>1.3285714285714201</v>
-      </c>
-      <c r="I29" t="s">
-        <v>324</v>
-      </c>
-      <c r="J29">
-        <v>-0.49964531245865501</v>
+        <v>832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>838</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H1:H30">
+    <sortCondition descending="1" ref="H1:H30"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in main figures.
</commit_message>
<xml_diff>
--- a/08_other_files/amps_tables.xlsx
+++ b/08_other_files/amps_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C25623A-2FE0-5647-B7A4-1D20C2BC54E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F717F127-5A29-7748-AE47-3354EF145E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{9D1A98CB-DC08-EA42-B350-3CAE810190DF}"/>
   </bookViews>
   <sheets>
     <sheet name="readcounts" sheetId="2" r:id="rId1"/>
@@ -36076,8 +36076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBC91AE-BB3C-D445-857D-BF013CB9D47D}">
   <dimension ref="A1:AA1096"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q28"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50213,7 +50213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB916D6-2511-874D-B076-27DA60C31731}">
   <dimension ref="A1:S194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>